<commit_message>
chg: Added SYTGT079 to tgt list
</commit_message>
<xml_diff>
--- a/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.4.xlsx
+++ b/INTELLIGENCE/TGT_LIST/OPAR v2.0_JOINT_TARGET_LIST_v1.4.xlsx
@@ -3017,7 +3017,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3051,7 +3051,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3275,9 +3275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5214,7 +5214,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A82" s="57" t="s">
+      <c r="A82" s="86" t="s">
         <v>694</v>
       </c>
       <c r="B82" s="18" t="s">
@@ -12888,9 +12888,10 @@
     <hyperlink ref="A61" r:id="rId54"/>
     <hyperlink ref="A64" r:id="rId55"/>
     <hyperlink ref="A140" r:id="rId56"/>
+    <hyperlink ref="A82" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId57"/>
-  <drawing r:id="rId58"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId58"/>
+  <drawing r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>